<commit_message>
Added mapping for Product Service Categories
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Open Sales Order Template_MFG FINAL.xlsx
+++ b/src/main/resources/templates/Open Sales Order Template_MFG FINAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Documents\DataProcessing\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD136B8-0DF8-41F6-BEED-4E3F9239AA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EF62A2-4F94-4B3D-8DDC-F7BEA83F527D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Restrictions" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="287">
   <si>
     <t>tranId</t>
   </si>
@@ -2245,6 +2245,21 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>productCategory</t>
+  </si>
+  <si>
+    <t>productCategoryID</t>
+  </si>
+  <si>
+    <t>Product Category</t>
+  </si>
+  <si>
+    <t>Product Category Internal ID</t>
+  </si>
+  <si>
+    <t>oldProductCategory</t>
   </si>
 </sst>
 </file>
@@ -4904,10 +4919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BX9"/>
+  <dimension ref="A1:CA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CA2" sqref="CA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4975,7 +4990,7 @@
     <col min="77" max="16384" width="31.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>249</v>
       </c>
@@ -5204,8 +5219,17 @@
       <c r="BX1" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="BY1" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="BZ1" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="CA1" s="23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>148</v>
       </c>
@@ -5434,8 +5458,14 @@
       <c r="BX2" s="23" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="3" spans="1:76" s="30" customFormat="1" ht="267.75" x14ac:dyDescent="0.2">
+      <c r="BY2" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="BZ2" s="23" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:79" s="30" customFormat="1" ht="267.75" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>153</v>
       </c>
@@ -5665,7 +5695,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>56</v>
       </c>
@@ -5887,7 +5917,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>149</v>
       </c>
@@ -6089,7 +6119,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:76" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:79" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>124</v>
       </c>
@@ -6187,7 +6217,7 @@
       <c r="BW6" s="14"/>
       <c r="BX6" s="14"/>
     </row>
-    <row r="7" spans="1:76" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:79" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>124</v>
       </c>
@@ -6285,7 +6315,7 @@
       <c r="BW7" s="14"/>
       <c r="BX7" s="14"/>
     </row>
-    <row r="8" spans="1:76" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:79" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>32</v>
       </c>
@@ -6363,7 +6393,7 @@
       <c r="BW8" s="8"/>
       <c r="BX8" s="27"/>
     </row>
-    <row r="9" spans="1:76" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:79" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>273</v>
       </c>

</xml_diff>